<commit_message>
roteiro de teste modal de opcionais
</commit_message>
<xml_diff>
--- a/TerceiroPasso/ModalOpcionais.xlsx
+++ b/TerceiroPasso/ModalOpcionais.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DTI DIGITAL\Desktop\DTI Digital\roteirosDeTeste\TerceiroPasso\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747F7983-4260-4F5F-9FD5-C06F093F499A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E08FFDB-161E-4F6C-A6A5-C5DF26F2791C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,12 +21,11 @@
     <sheet name="Qualidade" sheetId="6" r:id="rId6"/>
     <sheet name="Util" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="181029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -425,7 +424,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -551,6 +550,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -888,7 +894,7 @@
     <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1078,10 +1084,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1092,12 +1104,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1125,6 +1131,9 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -7497,10 +7506,10 @@
   <sheetPr>
     <tabColor rgb="FF376092"/>
   </sheetPr>
-  <dimension ref="A2:AMK12"/>
+  <dimension ref="A2:AMK19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -7585,10 +7594,10 @@
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="15" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7601,10 +7610,10 @@
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="15" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7619,10 +7628,10 @@
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="15" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7680,6 +7689,9 @@
       <c r="F12" s="15" t="s">
         <v>24</v>
       </c>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F19" s="88"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -8674,14 +8686,14 @@
       <c r="D1" s="24"/>
     </row>
     <row r="2" spans="1:19" ht="18" x14ac:dyDescent="0.25">
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="75" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B3" s="73" t="s">
+      <c r="B3" s="72" t="s">
         <v>64</v>
       </c>
       <c r="C3" s="25" t="s">
@@ -8692,7 +8704,7 @@
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="73"/>
+      <c r="B4" s="72"/>
       <c r="C4" t="s">
         <v>66</v>
       </c>
@@ -8701,7 +8713,7 @@
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="73"/>
+      <c r="B5" s="72"/>
       <c r="C5" s="27" t="s">
         <v>67</v>
       </c>
@@ -8710,7 +8722,7 @@
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B6" s="73"/>
+      <c r="B6" s="72"/>
       <c r="C6" s="27" t="s">
         <v>68</v>
       </c>
@@ -8719,12 +8731,12 @@
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="74"/>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
+      <c r="B7" s="76"/>
+      <c r="C7" s="76"/>
+      <c r="D7" s="76"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B8" s="75" t="s">
+      <c r="B8" s="77" t="s">
         <v>69</v>
       </c>
       <c r="C8" s="27" t="s">
@@ -8736,7 +8748,7 @@
       <c r="E8" s="24"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="75"/>
+      <c r="B9" s="77"/>
       <c r="C9" s="27" t="s">
         <v>71</v>
       </c>
@@ -8745,7 +8757,7 @@
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="75"/>
+      <c r="B10" s="77"/>
       <c r="C10" s="27" t="s">
         <v>72</v>
       </c>
@@ -8754,7 +8766,7 @@
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="75"/>
+      <c r="B11" s="77"/>
       <c r="C11" s="27" t="s">
         <v>73</v>
       </c>
@@ -8763,7 +8775,7 @@
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B12" s="75"/>
+      <c r="B12" s="77"/>
       <c r="C12" s="27" t="s">
         <v>74</v>
       </c>
@@ -8772,7 +8784,7 @@
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B13" s="75"/>
+      <c r="B13" s="77"/>
       <c r="C13" s="27" t="s">
         <v>75</v>
       </c>
@@ -8782,9 +8794,9 @@
     </row>
     <row r="14" spans="1:19" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="28"/>
-      <c r="B14" s="76"/>
-      <c r="C14" s="76"/>
-      <c r="D14" s="76"/>
+      <c r="B14" s="78"/>
+      <c r="C14" s="78"/>
+      <c r="D14" s="78"/>
       <c r="E14" s="28"/>
       <c r="F14" s="28"/>
       <c r="G14" s="28"/>
@@ -8802,7 +8814,7 @@
       <c r="S14" s="28"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B15" s="73" t="s">
+      <c r="B15" s="72" t="s">
         <v>76</v>
       </c>
       <c r="C15" s="27" t="s">
@@ -8814,7 +8826,7 @@
       <c r="E15" s="30"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B16" s="73"/>
+      <c r="B16" s="72"/>
       <c r="C16" s="27" t="s">
         <v>78</v>
       </c>
@@ -8823,12 +8835,12 @@
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="77"/>
-      <c r="C17" s="77"/>
-      <c r="D17" s="77"/>
+      <c r="B17" s="73"/>
+      <c r="C17" s="73"/>
+      <c r="D17" s="73"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="73" t="s">
+      <c r="B18" s="72" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="31" t="s">
@@ -8839,7 +8851,7 @@
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="73"/>
+      <c r="B19" s="72"/>
       <c r="C19" s="31" t="s">
         <v>80</v>
       </c>
@@ -8854,7 +8866,7 @@
       <c r="D20" s="34"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="73" t="s">
+      <c r="B21" s="72" t="s">
         <v>81</v>
       </c>
       <c r="C21" s="35" t="s">
@@ -8865,7 +8877,7 @@
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="73"/>
+      <c r="B22" s="72"/>
       <c r="C22" s="35" t="s">
         <v>83</v>
       </c>
@@ -8874,7 +8886,7 @@
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="73"/>
+      <c r="B23" s="72"/>
       <c r="C23" s="35" t="s">
         <v>84</v>
       </c>
@@ -8898,10 +8910,10 @@
       <c r="D26" s="38"/>
     </row>
     <row r="27" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B27" s="78" t="s">
+      <c r="B27" s="74" t="s">
         <v>85</v>
       </c>
-      <c r="C27" s="78"/>
+      <c r="C27" s="74"/>
       <c r="D27" s="39" t="s">
         <v>62</v>
       </c>
@@ -8918,16 +8930,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:B13"/>
+    <mergeCell ref="B14:D14"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="B21:B23"/>
     <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:B13"/>
-    <mergeCell ref="B14:D14"/>
   </mergeCells>
   <conditionalFormatting sqref="D8:D13 D18:D19 D3:D6 D15:D16">
     <cfRule type="cellIs" dxfId="43" priority="2" operator="equal">

</xml_diff>